<commit_message>
revised machine learning code & updated tableau visualisation uploaded
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\23. Project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\23. Project 3\Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D07F57E-D7EF-4F9E-AD84-4C19096B2D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC8ADB0-A54E-4A82-BBBA-0D91A8EDEA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Output</t>
   </si>
@@ -136,12 +136,6 @@
     <t xml:space="preserve">   Sub- bar/line chart on historical revenue</t>
   </si>
   <si>
-    <t xml:space="preserve">   Sub - Bubble Chart on successful bond movie (i.e Revenue, year, avg user rating)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Sub - line chart on age range of each bond movie?</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Sub - Martinis Drank</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">   Sub - Age Range</t>
-  </si>
-  <si>
-    <t>TBA</t>
   </si>
   <si>
     <t>Katherine, Kevin, Melissa, Cathy</t>
@@ -175,6 +166,15 @@
   </si>
   <si>
     <t>1. Web scraping on 25 movies?</t>
+  </si>
+  <si>
+    <t>Using Flask &amp; D3 visualisation on Bond Girls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sub - Scatter Plot on kill number vs revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Sub - Revenue per actor</t>
   </si>
 </sst>
 </file>
@@ -348,20 +348,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -371,31 +378,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -714,7 +714,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,19 +764,19 @@
         <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="20">
         <v>44511</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3" s="11">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,7 +788,9 @@
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11">
+        <v>0.8</v>
+      </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -802,7 +804,9 @@
       <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -816,95 +820,111 @@
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="37">
         <v>44515</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="31" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="37">
         <v>44515</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -912,15 +932,17 @@
         <v>25</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="38">
+        <v>35</v>
+      </c>
+      <c r="C15" s="26">
         <v>44516</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="11">
+        <v>0.5</v>
+      </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -928,26 +950,28 @@
         <v>29</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="38">
+      <c r="C16" s="26">
         <v>44516</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="27"/>
+      <c r="E16" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="38"/>
+        <v>40</v>
+      </c>
+      <c r="C17" s="26"/>
       <c r="D17" s="12"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="27" t="s">
         <v>14</v>
       </c>
     </row>
@@ -963,11 +987,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="E19" s="11"/>
       <c r="F19" s="8"/>
     </row>
@@ -1014,7 +1040,9 @@
       <c r="D24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="11">
+        <v>0.7</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,23 +1052,27 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0.7</v>
+      </c>
       <c r="F25" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0</v>
+      </c>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated machine learning code + tableau visualisation
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\23. Project 3\Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC8ADB0-A54E-4A82-BBBA-0D91A8EDEA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEB3D7D-8F16-4ABA-9DBD-A0FE6838E5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Output</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Best Bond actor? (maybe machine learning?)</t>
-  </si>
-  <si>
-    <t>Vote on James Bond next actor?</t>
   </si>
   <si>
     <t>Webpage visualisation on revenue as of 22 Nov 2021 with target revenue predicted by machine learning</t>
@@ -148,9 +145,6 @@
     <t>Katherine, Kevin, Melissa, Cathy</t>
   </si>
   <si>
-    <t>1. New python/JS library that does survey</t>
-  </si>
-  <si>
     <t>Hiroku Deployment</t>
   </si>
   <si>
@@ -162,12 +156,6 @@
     <t>James Bond Data set has been updated</t>
   </si>
   <si>
-    <t>Heat map on international sales based on country</t>
-  </si>
-  <si>
-    <t>1. Web scraping on 25 movies?</t>
-  </si>
-  <si>
     <t>Using Flask &amp; D3 visualisation on Bond Girls</t>
   </si>
   <si>
@@ -175,6 +163,13 @@
   </si>
   <si>
     <t xml:space="preserve">   Sub - Revenue per actor</t>
+  </si>
+  <si>
+    <t>Vote on James Bond next actor</t>
+  </si>
+  <si>
+    <t>1. New python/JS library that does survey
+2. Create a code that connects to database and update the database accordingly (stretch goal)</t>
   </si>
 </sst>
 </file>
@@ -303,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,7 +354,6 @@
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -711,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C11" sqref="C11:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,19 +758,19 @@
         <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="20">
         <v>44511</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="11">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,7 +783,7 @@
       <c r="C4" s="20"/>
       <c r="D4" s="12"/>
       <c r="E4" s="11">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F4" s="12"/>
     </row>
@@ -823,13 +817,13 @@
       <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="37">
+      <c r="B7" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="36">
         <v>44515</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11">
@@ -839,11 +833,11 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="29"/>
+        <v>29</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="11">
         <v>1</v>
       </c>
@@ -851,11 +845,11 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="29"/>
+        <v>38</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="11">
         <v>1</v>
       </c>
@@ -863,11 +857,11 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="11">
         <v>1</v>
       </c>
@@ -877,13 +871,13 @@
       <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="37">
+      <c r="B11" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="36">
         <v>44515</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="11">
@@ -893,11 +887,11 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="29"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="11">
         <v>1</v>
       </c>
@@ -905,11 +899,11 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="29"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="11">
         <v>1</v>
       </c>
@@ -917,22 +911,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="11">
         <v>1</v>
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" s="26">
         <v>44516</v>
@@ -941,13 +935,13 @@
         <v>5</v>
       </c>
       <c r="E15" s="11">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="26">
@@ -961,41 +955,37 @@
       </c>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="9"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -1013,82 +1003,74 @@
       <c r="E21" s="11"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="E24" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="12" t="s">
-        <v>6</v>
+      <c r="D25" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E25" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0</v>
-      </c>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <autoFilter ref="A1:F26" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
   <mergeCells count="6">
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="D11:D14"/>

</xml_diff>